<commit_message>
Add more commentary - MTurvey
</commit_message>
<xml_diff>
--- a/Data/Output/Output.xlsx
+++ b/Data/Output/Output.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailuc-my.sharepoint.com/personal/turveyms_mail_uc_edu/Documents/Documents/UiPath/RoboticEnterpriseFramework/Data/Output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailuc-my.sharepoint.com/personal/turveyms_mail_uc_edu/Documents/Documents/UiPath/Roboyo - Task Case/Data/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{3229D815-37D6-4D47-A541-692D6251E07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65D1C4F9-72D6-4328-919B-64209819D60B}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{3229D815-37D6-4D47-A541-692D6251E07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8115232-A354-4E8B-AE2D-2A3F65FBA34D}"/>
   <bookViews>
     <workbookView xWindow="6800" yWindow="1960" windowWidth="28800" windowHeight="15370" xr2:uid="{C7558A6F-66F6-48AA-A5B4-F03A18AF88CB}"/>
   </bookViews>
@@ -122,7 +122,7 @@
     <t>0912A</t>
   </si>
   <si>
-    <t>107,88€</t>
+    <t>107,82€</t>
   </si>
 </sst>
 </file>

</xml_diff>